<commit_message>
Update REgression test spreadsheet
</commit_message>
<xml_diff>
--- a/Doc/Regression Testing.xlsx
+++ b/Doc/Regression Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tang\Documents\GitHub\GMS2\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C65FD2-C90A-46C3-AA9B-1F5FA375609E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B43C65-6120-45FA-82BA-842CC1F8DD27}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{0BF8E5CF-0CEE-4673-A648-97D9790CFA54}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="121">
   <si>
     <t>Valid Cases</t>
   </si>
@@ -345,9 +345,6 @@
     <t>1324 Saltfield Road, City, NT, 1000</t>
   </si>
   <si>
-    <t>Issues  - Create an Account</t>
-  </si>
-  <si>
     <t>MMS_TC_S03</t>
   </si>
   <si>
@@ -385,13 +382,19 @@
   </si>
   <si>
     <t>Able to view calendar</t>
+  </si>
+  <si>
+    <t>Issues  - Create an Account - This has been resolved</t>
+  </si>
+  <si>
+    <t>Resolved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -439,14 +442,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -535,7 +530,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -549,11 +544,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -878,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91F0B04-3EBD-4EA0-A5F6-1A3CF0D2A22D}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,21 +897,21 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>102</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
-        <v>107</v>
+      <c r="A3" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>34</v>
@@ -951,8 +945,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
-        <v>108</v>
+      <c r="A4" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>34</v>
@@ -979,15 +973,15 @@
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L4" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
-        <v>109</v>
+      <c r="A5" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>34</v>
@@ -1021,8 +1015,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>110</v>
+      <c r="A6" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>34</v>
@@ -1056,8 +1050,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>111</v>
+      <c r="A7" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>34</v>
@@ -1091,8 +1085,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>112</v>
+      <c r="A8" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>34</v>
@@ -1126,24 +1120,24 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>113</v>
+      <c r="A9" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>114</v>
+      <c r="A10" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>116</v>
+      <c r="A11" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>34</v>
@@ -1386,8 +1380,8 @@
       <c r="I23" t="s">
         <v>96</v>
       </c>
-      <c r="J23" s="12" t="s">
-        <v>76</v>
+      <c r="J23" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="K23" t="s">
         <v>94</v>
@@ -1586,8 +1580,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>106</v>
+      <c r="A32" s="7" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>